<commit_message>
Important report related updates and the GUI general viewing upgrades
</commit_message>
<xml_diff>
--- a/11b_IMS_System_Data/3_Invoice/Invoice # 002.xlsx
+++ b/11b_IMS_System_Data/3_Invoice/Invoice # 002.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repos\CSharp\IMS_System_Data\3_Invoice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\CSharp\11b_IMS_System_DATA\3_Invoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDE0932-4D35-422F-9CD5-8819E192D50F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice No. 002" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -88,9 +87,6 @@
     <t>sibte.5shah@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Previous payment as per Invoice # : </t>
-  </si>
-  <si>
     <t xml:space="preserve">SUBTOTAL LESS DISCOUNT: </t>
   </si>
   <si>
@@ -104,16 +100,6 @@
   </si>
   <si>
     <t>BILL TO:</t>
-  </si>
-  <si>
-    <t>Inventory Management System (IMS) in MS Excel to be finalized based on the latest MoU including below items:
-- Full customer/supplier invoice entry
-- Import customer/supplier invoices
-- Import customer/supplier/product list records
-- Re-order levels
-- Report on Stocks
-- Report on re-order levels
-- Detailed product sale/purchase history</t>
   </si>
   <si>
     <t>PAYMENT DEAILS:</t>
@@ -137,24 +123,38 @@
     </r>
   </si>
   <si>
-    <t>31 - 01 - 2020</t>
-  </si>
-  <si>
     <t xml:space="preserve"> # 002</t>
   </si>
   <si>
     <t xml:space="preserve">Final Invoice: </t>
+  </si>
+  <si>
+    <t>06 - 03 - 2020</t>
+  </si>
+  <si>
+    <t>Inventory Management System (IMS) as GUI Desktop Program with below capabilities:
+- Login Screen for Admin Access
+- Full customer/supplier invoice entry
+- Import customer/supplier invoices
+- Import customer/supplier/product list records
+- Re-order levels
+- Report on Stocks
+- Report on re-order levels
+- Detailed product sale/purchase history</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous payment as per Invoice # 1 : </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@"/>
   </numFmts>
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="44">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -793,53 +793,20 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="40" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -848,6 +815,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -870,8 +840,38 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
-    <xf numFmtId="2" fontId="40" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1187,7 +1187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF8496B0"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -1195,11 +1195,11 @@
   </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
@@ -1212,7 +1212,7 @@
     <col min="9" max="9" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="27" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -1223,37 +1223,37 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="32.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="87" t="s">
+      <c r="C2" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="88"/>
+      <c r="D2" s="78"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="67"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="18.75" customHeight="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="86" t="s">
+      <c r="B3" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="7"/>
       <c r="G3" s="6"/>
       <c r="H3" s="8"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="18" customHeight="1">
       <c r="A4" s="6"/>
-      <c r="B4" s="66"/>
+      <c r="B4" s="67"/>
       <c r="C4" s="53" t="s">
         <v>12</v>
       </c>
@@ -1264,9 +1264,9 @@
       <c r="H4" s="12"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="18" customHeight="1">
       <c r="A5" s="6"/>
-      <c r="B5" s="66"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="10"/>
       <c r="D5" s="1"/>
       <c r="E5" s="14"/>
@@ -1275,9 +1275,9 @@
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
     </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="18" customHeight="1">
       <c r="A6" s="6"/>
-      <c r="B6" s="66"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="10"/>
       <c r="D6" s="1"/>
       <c r="E6" s="11"/>
@@ -1286,11 +1286,11 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="18" customHeight="1">
       <c r="A7" s="6"/>
-      <c r="B7" s="66"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="11"/>
@@ -1299,17 +1299,17 @@
       <c r="H7" s="18"/>
       <c r="I7" s="19"/>
     </row>
-    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="18" customHeight="1">
       <c r="A8" s="6"/>
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="83" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="55" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="66"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="67"/>
       <c r="G8" s="56" t="s">
         <v>1</v>
       </c>
@@ -1318,98 +1318,98 @@
       </c>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="18" customHeight="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="66"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="51" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="66"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="21"/>
       <c r="H9" s="22"/>
       <c r="I9" s="23"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1">
       <c r="A10" s="6"/>
-      <c r="B10" s="66"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="54" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="66"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="67"/>
       <c r="G10" s="24"/>
       <c r="H10" s="25"/>
       <c r="I10" s="25"/>
     </row>
-    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="18" customHeight="1">
       <c r="A11" s="6"/>
-      <c r="B11" s="66"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="20"/>
       <c r="D11" s="26"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="66"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="67"/>
       <c r="G11" s="24"/>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
     </row>
-    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="18" customHeight="1">
       <c r="A12" s="6"/>
-      <c r="B12" s="66"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="20"/>
       <c r="D12" s="26"/>
       <c r="G12" s="27"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="18" customHeight="1">
       <c r="A13" s="6"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="92" t="s">
+      <c r="B13" s="67"/>
+      <c r="C13" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="85"/>
+      <c r="D13" s="74"/>
       <c r="E13" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="84" t="s">
+      <c r="F13" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="85"/>
+      <c r="G13" s="74"/>
       <c r="H13" s="29" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="126.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="126.75" customHeight="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="90" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="91"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="81"/>
       <c r="E14" s="30">
-        <v>54</v>
-      </c>
-      <c r="F14" s="82">
+        <v>68</v>
+      </c>
+      <c r="F14" s="71">
         <v>40</v>
       </c>
-      <c r="G14" s="83"/>
+      <c r="G14" s="72"/>
       <c r="H14" s="31">
         <f t="shared" ref="H14:H17" si="0">E14*F14</f>
-        <v>2160</v>
+        <v>2720</v>
       </c>
       <c r="I14" s="32"/>
     </row>
-    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="18" customHeight="1">
       <c r="A15" s="6"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="73"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="69"/>
       <c r="D15" s="70"/>
       <c r="E15" s="33"/>
-      <c r="F15" s="69"/>
+      <c r="F15" s="75"/>
       <c r="G15" s="70"/>
       <c r="H15" s="31">
         <f t="shared" si="0"/>
@@ -1417,13 +1417,13 @@
       </c>
       <c r="I15" s="32"/>
     </row>
-    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="18" customHeight="1">
       <c r="A16" s="6"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="69"/>
       <c r="D16" s="70"/>
       <c r="E16" s="33"/>
-      <c r="F16" s="69"/>
+      <c r="F16" s="75"/>
       <c r="G16" s="70"/>
       <c r="H16" s="31">
         <f t="shared" si="0"/>
@@ -1431,13 +1431,13 @@
       </c>
       <c r="I16" s="32"/>
     </row>
-    <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="18" customHeight="1">
       <c r="A17" s="6"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="74"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="89"/>
       <c r="D17" s="70"/>
       <c r="E17" s="34"/>
-      <c r="F17" s="71"/>
+      <c r="F17" s="87"/>
       <c r="G17" s="70"/>
       <c r="H17" s="31">
         <f t="shared" si="0"/>
@@ -1445,27 +1445,27 @@
       </c>
       <c r="I17" s="32"/>
     </row>
-    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="19.5" customHeight="1">
       <c r="A18" s="6"/>
-      <c r="B18" s="66"/>
+      <c r="B18" s="67"/>
       <c r="C18" s="61" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="36"/>
       <c r="F18" s="36"/>
       <c r="G18" s="37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" s="38">
         <f>SUM(H14:H17)</f>
-        <v>2160</v>
+        <v>2720</v>
       </c>
       <c r="I18" s="39"/>
     </row>
-    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="19.5" customHeight="1">
       <c r="A19" s="6"/>
-      <c r="B19" s="66"/>
+      <c r="B19" s="67"/>
       <c r="C19" s="52" t="s">
         <v>11</v>
       </c>
@@ -1473,67 +1473,67 @@
       <c r="E19" s="36"/>
       <c r="F19" s="36"/>
       <c r="G19" s="40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H19" s="38">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="I19" s="39"/>
     </row>
-    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="19.5" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="79" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="79"/>
+      <c r="C20" s="94" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="94"/>
       <c r="E20" s="59"/>
       <c r="F20" s="36"/>
       <c r="G20" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H20" s="38">
         <f>H18-H19</f>
-        <v>2060</v>
+        <v>2520</v>
       </c>
       <c r="I20" s="39"/>
     </row>
-    <row r="21" spans="1:9" s="58" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="58" customFormat="1" ht="19.5" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="94"/>
       <c r="E21" s="59"/>
       <c r="F21" s="36"/>
       <c r="G21" s="63" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H21" s="62">
         <v>890</v>
       </c>
       <c r="I21" s="39"/>
     </row>
-    <row r="22" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="19.5" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="5"/>
-      <c r="C22" s="79"/>
-      <c r="D22" s="79"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
       <c r="E22" s="59"/>
       <c r="F22" s="36"/>
       <c r="G22" s="64" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="94">
+        <v>23</v>
+      </c>
+      <c r="H22" s="65">
         <f>H20-H21</f>
-        <v>1170</v>
+        <v>1630</v>
       </c>
       <c r="I22" s="41"/>
     </row>
-    <row r="23" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="33.75" customHeight="1">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="66"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="67"/>
       <c r="E23" s="36"/>
       <c r="F23" s="36"/>
       <c r="G23" s="42" t="s">
@@ -1541,29 +1541,29 @@
       </c>
       <c r="H23" s="43">
         <f>H22</f>
-        <v>1170</v>
+        <v>1630</v>
       </c>
       <c r="I23" s="44"/>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="6"/>
       <c r="B24" s="5"/>
-      <c r="C24" s="67" t="str">
+      <c r="C24" s="85" t="str">
         <f>"as per this "&amp;B8&amp;B3</f>
         <v>as per this INVOICE # 002</v>
       </c>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
       <c r="I24" s="45"/>
     </row>
-    <row r="25" spans="1:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="9.75" customHeight="1">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
       <c r="C25" s="46" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
@@ -1572,42 +1572,42 @@
       <c r="H25" s="45"/>
       <c r="I25" s="45"/>
     </row>
-    <row r="26" spans="1:9" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="44.25" customHeight="1">
       <c r="A26" s="6"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="77" t="s">
-        <v>22</v>
-      </c>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="78"/>
-      <c r="G26" s="78"/>
-      <c r="H26" s="78"/>
+      <c r="C26" s="92" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="93"/>
+      <c r="E26" s="93"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="93"/>
+      <c r="H26" s="93"/>
       <c r="I26" s="47"/>
     </row>
-    <row r="27" spans="1:9" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="10.5" customHeight="1">
       <c r="A27" s="6"/>
       <c r="B27" s="5"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
-      <c r="G27" s="76"/>
-      <c r="H27" s="76"/>
+      <c r="C27" s="90"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="91"/>
+      <c r="G27" s="91"/>
+      <c r="H27" s="91"/>
       <c r="I27" s="48"/>
     </row>
-    <row r="28" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="21" customHeight="1">
       <c r="A28" s="49"/>
       <c r="B28" s="49"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="67"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
       <c r="I28" s="50"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15.75" customHeight="1">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -1620,6 +1620,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C20:D22"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="C15:D15"/>
@@ -1635,19 +1645,9 @@
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="B8:B19"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C24:H24"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C20:D22"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C10" r:id="rId1"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>